<commit_message>
Remove buffer and patch tube casing
</commit_message>
<xml_diff>
--- a/tests/fixtures/orderforms/pacbio_revio_sequencing_1.xlsx
+++ b/tests/fixtures/orderforms/pacbio_revio_sequencing_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10916"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christian/Documents/clinicalGenomics/cg/tests/fixtures/orderforms/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isakohlsson/dev/cg/tests/fixtures/orderforms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD9A0E6F-6E0C-F144-B897-193DFB4C882B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85E132B1-57A2-054B-B7BF-86B03F24B3CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16240" tabRatio="993" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="500" windowWidth="51200" windowHeight="28300" tabRatio="993" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="information" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="414">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="413">
   <si>
     <t>https://clinical.scilifelab.se/</t>
   </si>
@@ -1730,10 +1730,7 @@
     <t>BAM</t>
   </si>
   <si>
-    <t>pacbio_test_sample</t>
-  </si>
-  <si>
-    <t>tube</t>
+    <t>PacbioTestSample</t>
   </si>
 </sst>
 </file>
@@ -3158,7 +3155,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
@@ -3370,8 +3367,8 @@
   </sheetPr>
   <dimension ref="A1:ALT395"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView showGridLines="0" topLeftCell="A2" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" outlineLevelRow="1" x14ac:dyDescent="0.15"/>
@@ -10707,7 +10704,7 @@
         <v>1234</v>
       </c>
       <c r="L15" s="66" t="s">
-        <v>413</v>
+        <v>45</v>
       </c>
       <c r="M15" s="43"/>
       <c r="N15" s="57"/>

</xml_diff>

<commit_message>
Remove buffer and patch tube casing and add well position (#3953) (patch)
### Fixed

- buffer is removed as a field from the PacbioSample
- The test fixture for a pacbio order form has been patched.
</commit_message>
<xml_diff>
--- a/tests/fixtures/orderforms/pacbio_revio_sequencing_1.xlsx
+++ b/tests/fixtures/orderforms/pacbio_revio_sequencing_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10916"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christian/Documents/clinicalGenomics/cg/tests/fixtures/orderforms/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isakohlsson/dev/cg/tests/fixtures/orderforms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD9A0E6F-6E0C-F144-B897-193DFB4C882B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85E132B1-57A2-054B-B7BF-86B03F24B3CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16240" tabRatio="993" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="500" windowWidth="51200" windowHeight="28300" tabRatio="993" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="information" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="414">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="413">
   <si>
     <t>https://clinical.scilifelab.se/</t>
   </si>
@@ -1730,10 +1730,7 @@
     <t>BAM</t>
   </si>
   <si>
-    <t>pacbio_test_sample</t>
-  </si>
-  <si>
-    <t>tube</t>
+    <t>PacbioTestSample</t>
   </si>
 </sst>
 </file>
@@ -3158,7 +3155,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
@@ -3370,8 +3367,8 @@
   </sheetPr>
   <dimension ref="A1:ALT395"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView showGridLines="0" topLeftCell="A2" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" outlineLevelRow="1" x14ac:dyDescent="0.15"/>
@@ -10707,7 +10704,7 @@
         <v>1234</v>
       </c>
       <c r="L15" s="66" t="s">
-        <v>413</v>
+        <v>45</v>
       </c>
       <c r="M15" s="43"/>
       <c r="N15" s="57"/>

</xml_diff>